<commit_message>
aggiornamento analisi dei rischi
aggiornamento analisi dei rischi con nuovi rischi
</commit_message>
<xml_diff>
--- a/analisi dei rischi/analisiDeiRiscihiEXCEL.xlsx
+++ b/analisi dei rischi/analisiDeiRiscihiEXCEL.xlsx
@@ -5,10 +5,10 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Desktop\progettoGestione\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\Download\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5AB8076-F03F-4E92-A684-7CF5BF3CF610}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC186F31-8655-4F50-BED9-9334B94560CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12105" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t xml:space="preserve">Any articles, templates, or information provided by Smartsheet on the website are for reference only. While we strive to keep the information up to date and correct, we make no representations or warranties of any kind, express or implied, about the completeness, accuracy, reliability, suitability, or availability with respect to the website or the information, articles, templates, or related graphics contained on the website. Any reliance you place on such information is therefore strictly at your own risk. </t>
   </si>
@@ -75,9 +75,6 @@
     <t>Minacce alla Sicurezza e Accessi Non Autorizzati</t>
   </si>
   <si>
-    <t>Difficoltà nell'Integrazione con Altri Sistemi</t>
-  </si>
-  <si>
     <t>Complessità nell'Implementazione dell'Intelligenza Artificiale</t>
   </si>
   <si>
@@ -151,6 +148,54 @@
   </si>
   <si>
     <t>Valutazione costante delle esigenze degli utenti per apportare modifiche.</t>
+  </si>
+  <si>
+    <t>Difficoltà nell'Integrazione con Altri Sistemi proprietari</t>
+  </si>
+  <si>
+    <t>Disponibilità limitata dell’azienda per gli incontri con il team di sviluppo della scuola</t>
+  </si>
+  <si>
+    <t>Superamento del Budget Allocato</t>
+  </si>
+  <si>
+    <t>Ritardi e problemi di comunicabilità con la Limonta s.p.a</t>
+  </si>
+  <si>
+    <t>Comunicazione</t>
+  </si>
+  <si>
+    <t>Costo</t>
+  </si>
+  <si>
+    <t>Alto</t>
+  </si>
+  <si>
+    <t>medio</t>
+  </si>
+  <si>
+    <t>Possibili ritardi e problemi di comunicazione con la Limonta s.p.a possono ostacolare il flusso di informazioni vitali per lo sviluppo del progetto.</t>
+  </si>
+  <si>
+    <t>La disponibilità limitata dell'azienda per incontri con il team di sviluppo della scuola potrebbe ostacolare la collaborazione e la comprensione reciproca.</t>
+  </si>
+  <si>
+    <t>Implementare canali di comunicazione chiari con la Limonta s.p.a, pianificare incontri regolari per monitorare lo stato del progetto e risolvere tempestivamente eventuali problemi di comunicazione. Assicurarsi che le informazioni vitali siano trasmesse in modo efficiente tra le parti coinvolte.</t>
+  </si>
+  <si>
+    <t>Implementazione di canali di comunicazione. Pianificazione di incontri regolari.</t>
+  </si>
+  <si>
+    <t>Monitoraggio costante dei costi del progetto.</t>
+  </si>
+  <si>
+    <t>Pianificazione flessibile degli incontri per adattarsi alla disponibilità dell'azienda.</t>
+  </si>
+  <si>
+    <t>Monitorare costantemente i costi del progetto, implementare controlli finanziari e di budget. Pianificare riserve finanziarie per affrontare eventuali imprevisti. Adottare pratiche di gestione finanziaria oculate per mantenere il progetto all'interno dei limiti di spesa previsti.</t>
+  </si>
+  <si>
+    <t>Adottare una pianificazione flessibile degli incontri per adattarsi alla disponibilità dell'azienda. Utilizzare mezzi di comunicazione virtuali quando possibile per ridurre la dipendenza dagli incontri fisici. Mantenere una comunicazione regolare attraverso documentazione chiara e aggiornamenti periodici, garantendo che tutte le informazioni rilevanti siano condivise in modo efficace.</t>
   </si>
 </sst>
 </file>
@@ -331,7 +376,100 @@
     <cellStyle name="Normal 2" xfId="1" xr:uid="{A9DF3BC1-9742-6741-902A-E2056DAAB984}"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -771,7 +909,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -783,8 +921,8 @@
     <col min="5" max="5" width="25.875" style="2" customWidth="1"/>
     <col min="6" max="6" width="18.875" style="2" customWidth="1"/>
     <col min="7" max="7" width="45.75" style="2" customWidth="1"/>
-    <col min="8" max="8" width="20.75" style="2" customWidth="1"/>
-    <col min="9" max="9" width="27.875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="35.5" style="2" customWidth="1"/>
+    <col min="9" max="9" width="46.875" style="2" customWidth="1"/>
     <col min="10" max="10" width="25.875" style="2" customWidth="1"/>
     <col min="11" max="12" width="11.875" style="2" customWidth="1"/>
     <col min="13" max="13" width="18.875" style="2" customWidth="1"/>
@@ -835,7 +973,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" s="12" t="s">
         <v>7</v>
@@ -857,22 +995,22 @@
         <v>9</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="13">
         <v>3</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J3"/>
       <c r="K3"/>
@@ -888,22 +1026,22 @@
         <v>10</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F4" s="13">
         <v>2</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4"/>
@@ -919,22 +1057,22 @@
         <v>11</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F5" s="13">
         <v>3</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5"/>
@@ -950,22 +1088,22 @@
         <v>12</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F6" s="13">
         <v>3</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6"/>
@@ -978,25 +1116,25 @@
         <v>5</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="D7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>20</v>
       </c>
       <c r="F7" s="13">
         <v>2</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7"/>
@@ -1009,25 +1147,25 @@
         <v>6</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" s="13">
         <v>2</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8"/>
@@ -1040,25 +1178,25 @@
         <v>7</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" s="13">
         <v>2</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I9" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9"/>
@@ -1066,45 +1204,93 @@
       <c r="M9"/>
       <c r="N9"/>
     </row>
-    <row r="10" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+    <row r="10" spans="1:14" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="11">
+        <v>8</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="13">
+        <v>3</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>48</v>
+      </c>
       <c r="J10" s="4"/>
       <c r="K10"/>
       <c r="L10"/>
       <c r="M10"/>
       <c r="N10"/>
     </row>
-    <row r="11" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+    <row r="11" spans="1:14" ht="91.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="11">
+        <v>9</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="13">
+        <v>2</v>
+      </c>
+      <c r="G11" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>52</v>
+      </c>
       <c r="J11" s="4"/>
       <c r="K11"/>
       <c r="L11"/>
       <c r="M11"/>
       <c r="N11"/>
     </row>
-    <row r="12" spans="1:14" ht="24.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
+    <row r="12" spans="1:14" ht="139.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="11">
+        <v>10</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="13">
+        <v>3</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>53</v>
+      </c>
       <c r="J12" s="4"/>
       <c r="K12"/>
       <c r="L12"/>
@@ -1338,51 +1524,84 @@
     <row r="36" ht="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <conditionalFormatting sqref="F3:G9">
-    <cfRule type="containsText" dxfId="11" priority="27" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="20" priority="36" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="28" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="19" priority="37" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",F3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="29" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="18" priority="38" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",F3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="17" priority="16" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",H3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="15" priority="18" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4:H9">
-    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="3">
+    <cfRule type="containsText" dxfId="14" priority="13" operator="containsText" text="3">
       <formula>NOT(ISERROR(SEARCH("3",H4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="2">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="2">
       <formula>NOT(ISERROR(SEARCH("2",H4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="1">
+    <cfRule type="containsText" dxfId="12" priority="15" operator="containsText" text="1">
       <formula>NOT(ISERROR(SEARCH("1",H4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3:I9">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="3">
+      <formula>NOT(ISERROR(SEARCH("3",I3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="2">
+      <formula>NOT(ISERROR(SEARCH("2",I3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="12" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",I3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="3">
+      <formula>NOT(ISERROR(SEARCH("3",F10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="2">
+      <formula>NOT(ISERROR(SEARCH("2",F10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="9" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",F10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="3">
+      <formula>NOT(ISERROR(SEARCH("3",F12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="2">
+      <formula>NOT(ISERROR(SEARCH("2",F12)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="1">
+      <formula>NOT(ISERROR(SEARCH("1",F12)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F11">
     <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="3">
-      <formula>NOT(ISERROR(SEARCH("3",I3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("3",F11)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="2">
-      <formula>NOT(ISERROR(SEARCH("2",I3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("2",F11)))</formula>
     </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="1">
-      <formula>NOT(ISERROR(SEARCH("1",I3)))</formula>
+      <formula>NOT(ISERROR(SEARCH("1",F11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G20:G26 F3:F19" xr:uid="{5842BFDF-4532-604E-8573-6BC2D9D427C0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G20:G26 F3:F9 F13:F19" xr:uid="{5842BFDF-4532-604E-8573-6BC2D9D427C0}">
       <formula1>#REF!</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H20:H26 G3:G19" xr:uid="{8ADB8308-C53A-E749-AB9F-E096A234902B}">

</xml_diff>